<commit_message>
Copy Paste Feature(Engage) & Test Invitation(All Three Servers)
</commit_message>
<xml_diff>
--- a/Engage/Research-Smoke/src/main/resources/excelfiles/Research_Smoke.xlsx
+++ b/Engage/Research-Smoke/src/main/resources/excelfiles/Research_Smoke.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="506">
   <si>
     <t>Environment</t>
   </si>
@@ -1181,9 +1181,6 @@
     <t>Smoke_TC74</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Create Project Button not present on page.</t>
   </si>
   <si>
@@ -1579,6 +1576,57 @@
   </si>
   <si>
     <t>Anas</t>
+  </si>
+  <si>
+    <t>Smoke_TC75</t>
+  </si>
+  <si>
+    <t>Test Invite</t>
+  </si>
+  <si>
+    <t>Send Test Invitations</t>
+  </si>
+  <si>
+    <t>Test Invite Sample TextBox</t>
+  </si>
+  <si>
+    <t>g_golatkar@outlook.com</t>
+  </si>
+  <si>
+    <t>TestInvite</t>
+  </si>
+  <si>
+    <t>Default Classic System Defined Email</t>
+  </si>
+  <si>
+    <t>selectET_1</t>
+  </si>
+  <si>
+    <t>outlook</t>
+  </si>
+  <si>
+    <t>gvg3196@test</t>
+  </si>
+  <si>
+    <t>Your Voice Counts</t>
+  </si>
+  <si>
+    <t>SelectTemplate</t>
+  </si>
+  <si>
+    <t>emailhost</t>
+  </si>
+  <si>
+    <t>stremailaddress</t>
+  </si>
+  <si>
+    <t>emailPassword</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -1759,7 +1807,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1795,9 +1843,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="4" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2298,10 +2353,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CP63"/>
+  <dimension ref="A1:CU64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,7 +2381,7 @@
     <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -2355,7 +2410,7 @@
         <v>10</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>21</v>
@@ -2609,8 +2664,23 @@
       <c r="CP1" s="3" t="s">
         <v>208</v>
       </c>
+      <c r="CQ1" s="35" t="s">
+        <v>500</v>
+      </c>
+      <c r="CR1" s="35" t="s">
+        <v>501</v>
+      </c>
+      <c r="CS1" s="35" t="s">
+        <v>502</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>504</v>
+      </c>
     </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -2633,7 +2703,7 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J2" s="4"/>
@@ -2723,8 +2793,13 @@
       <c r="CN2" s="6"/>
       <c r="CO2" s="6"/>
       <c r="CP2" s="6"/>
+      <c r="CQ2" s="1"/>
+      <c r="CR2" s="1"/>
+      <c r="CS2" s="1"/>
+      <c r="CT2" s="1"/>
+      <c r="CU2" s="1"/>
     </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -2747,8 +2822,8 @@
       <c r="H3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="33" t="s">
-        <v>365</v>
+      <c r="I3" s="40" t="s">
+        <v>173</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>324</v>
@@ -2917,8 +2992,13 @@
       <c r="CN3" s="6"/>
       <c r="CO3" s="6"/>
       <c r="CP3" s="6"/>
+      <c r="CQ3" s="1"/>
+      <c r="CR3" s="1"/>
+      <c r="CS3" s="1"/>
+      <c r="CT3" s="1"/>
+      <c r="CU3" s="1"/>
     </row>
-    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>182</v>
       </c>
@@ -2941,7 +3021,7 @@
       <c r="H4" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J4" s="11" t="s">
@@ -3045,8 +3125,13 @@
       </c>
       <c r="CO4" s="25"/>
       <c r="CP4" s="25"/>
+      <c r="CQ4" s="1"/>
+      <c r="CR4" s="1"/>
+      <c r="CS4" s="1"/>
+      <c r="CT4" s="1"/>
+      <c r="CU4" s="1"/>
     </row>
-    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>183</v>
       </c>
@@ -3069,7 +3154,7 @@
       <c r="H5" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J5" s="11"/>
@@ -3171,8 +3256,13 @@
       </c>
       <c r="CO5" s="15"/>
       <c r="CP5" s="15"/>
+      <c r="CQ5" s="1"/>
+      <c r="CR5" s="1"/>
+      <c r="CS5" s="1"/>
+      <c r="CT5" s="1"/>
+      <c r="CU5" s="1"/>
     </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>184</v>
       </c>
@@ -3195,7 +3285,7 @@
       <c r="H6" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J6" s="11"/>
@@ -3287,8 +3377,13 @@
       <c r="CN6" s="15"/>
       <c r="CO6" s="15"/>
       <c r="CP6" s="15"/>
+      <c r="CQ6" s="1"/>
+      <c r="CR6" s="1"/>
+      <c r="CS6" s="1"/>
+      <c r="CT6" s="1"/>
+      <c r="CU6" s="1"/>
     </row>
-    <row r="7" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>185</v>
       </c>
@@ -3311,7 +3406,7 @@
       <c r="H7" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J7" s="11" t="s">
@@ -3407,8 +3502,13 @@
       <c r="CN7" s="15"/>
       <c r="CO7" s="15"/>
       <c r="CP7" s="15"/>
+      <c r="CQ7" s="1"/>
+      <c r="CR7" s="1"/>
+      <c r="CS7" s="1"/>
+      <c r="CT7" s="1"/>
+      <c r="CU7" s="1"/>
     </row>
-    <row r="8" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>186</v>
       </c>
@@ -3431,7 +3531,7 @@
       <c r="H8" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J8" s="11"/>
@@ -3525,8 +3625,13 @@
       <c r="CN8" s="15"/>
       <c r="CO8" s="15"/>
       <c r="CP8" s="15"/>
+      <c r="CQ8" s="1"/>
+      <c r="CR8" s="1"/>
+      <c r="CS8" s="1"/>
+      <c r="CT8" s="1"/>
+      <c r="CU8" s="1"/>
     </row>
-    <row r="9" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>187</v>
       </c>
@@ -3547,7 +3652,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J9" s="1"/>
@@ -3649,8 +3754,13 @@
       </c>
       <c r="CO9" s="13"/>
       <c r="CP9" s="13"/>
+      <c r="CQ9" s="1"/>
+      <c r="CR9" s="1"/>
+      <c r="CS9" s="1"/>
+      <c r="CT9" s="1"/>
+      <c r="CU9" s="1"/>
     </row>
-    <row r="10" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>188</v>
       </c>
@@ -3673,8 +3783,8 @@
         <v>191</v>
       </c>
       <c r="H10" s="17"/>
-      <c r="I10" s="34" t="s">
-        <v>173</v>
+      <c r="I10" s="39" t="s">
+        <v>505</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>321</v>
@@ -3775,8 +3885,13 @@
       <c r="CP10" s="19" t="s">
         <v>209</v>
       </c>
+      <c r="CQ10" s="1"/>
+      <c r="CR10" s="1"/>
+      <c r="CS10" s="1"/>
+      <c r="CT10" s="1"/>
+      <c r="CU10" s="1"/>
     </row>
-    <row r="11" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>193</v>
       </c>
@@ -3799,8 +3914,8 @@
         <v>195</v>
       </c>
       <c r="H11" s="17"/>
-      <c r="I11" s="34" t="s">
-        <v>173</v>
+      <c r="I11" s="39" t="s">
+        <v>505</v>
       </c>
       <c r="J11" s="18" t="s">
         <v>318</v>
@@ -3897,8 +4012,13 @@
       <c r="CP11" s="19" t="s">
         <v>209</v>
       </c>
+      <c r="CQ11" s="1"/>
+      <c r="CR11" s="1"/>
+      <c r="CS11" s="1"/>
+      <c r="CT11" s="1"/>
+      <c r="CU11" s="1"/>
     </row>
-    <row r="12" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>197</v>
       </c>
@@ -3921,8 +4041,8 @@
         <v>199</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="34" t="s">
-        <v>173</v>
+      <c r="I12" s="39" t="s">
+        <v>505</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>318</v>
@@ -4019,8 +4139,13 @@
       <c r="CP12" s="19" t="s">
         <v>209</v>
       </c>
+      <c r="CQ12" s="1"/>
+      <c r="CR12" s="1"/>
+      <c r="CS12" s="1"/>
+      <c r="CT12" s="1"/>
+      <c r="CU12" s="1"/>
     </row>
-    <row r="13" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>201</v>
       </c>
@@ -4043,8 +4168,8 @@
         <v>203</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="34" t="s">
-        <v>173</v>
+      <c r="I13" s="39" t="s">
+        <v>505</v>
       </c>
       <c r="J13" s="18" t="s">
         <v>318</v>
@@ -4141,8 +4266,13 @@
       <c r="CP13" s="19" t="s">
         <v>209</v>
       </c>
+      <c r="CQ13" s="1"/>
+      <c r="CR13" s="1"/>
+      <c r="CS13" s="1"/>
+      <c r="CT13" s="1"/>
+      <c r="CU13" s="1"/>
     </row>
-    <row r="14" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>205</v>
       </c>
@@ -4165,8 +4295,8 @@
         <v>207</v>
       </c>
       <c r="H14" s="21"/>
-      <c r="I14" s="34" t="s">
-        <v>173</v>
+      <c r="I14" s="39" t="s">
+        <v>505</v>
       </c>
       <c r="J14" s="22" t="s">
         <v>318</v>
@@ -4263,8 +4393,13 @@
       <c r="CP14" s="23" t="s">
         <v>209</v>
       </c>
+      <c r="CQ14" s="1"/>
+      <c r="CR14" s="1"/>
+      <c r="CS14" s="1"/>
+      <c r="CT14" s="1"/>
+      <c r="CU14" s="1"/>
     </row>
-    <row r="15" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>217</v>
       </c>
@@ -4287,7 +4422,7 @@
       <c r="H15" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J15" s="11" t="s">
@@ -4391,8 +4526,13 @@
       </c>
       <c r="CO15" s="25"/>
       <c r="CP15" s="25"/>
+      <c r="CQ15" s="1"/>
+      <c r="CR15" s="1"/>
+      <c r="CS15" s="1"/>
+      <c r="CT15" s="1"/>
+      <c r="CU15" s="1"/>
     </row>
-    <row r="16" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>220</v>
       </c>
@@ -4413,8 +4553,8 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="34" t="s">
-        <v>173</v>
+      <c r="I16" s="39" t="s">
+        <v>505</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="1"/>
@@ -4507,8 +4647,13 @@
       <c r="CN16" s="25"/>
       <c r="CO16" s="25"/>
       <c r="CP16" s="25"/>
+      <c r="CQ16" s="1"/>
+      <c r="CR16" s="1"/>
+      <c r="CS16" s="1"/>
+      <c r="CT16" s="1"/>
+      <c r="CU16" s="1"/>
     </row>
-    <row r="17" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>225</v>
       </c>
@@ -4529,8 +4674,8 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="34" t="s">
-        <v>173</v>
+      <c r="I17" s="39" t="s">
+        <v>505</v>
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="1"/>
@@ -4623,8 +4768,13 @@
       <c r="CN17" s="25"/>
       <c r="CO17" s="25"/>
       <c r="CP17" s="25"/>
+      <c r="CQ17" s="1"/>
+      <c r="CR17" s="1"/>
+      <c r="CS17" s="1"/>
+      <c r="CT17" s="1"/>
+      <c r="CU17" s="1"/>
     </row>
-    <row r="18" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>231</v>
       </c>
@@ -4647,7 +4797,7 @@
         <v>274</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J18" s="26"/>
@@ -4745,8 +4895,13 @@
       <c r="CN18" s="25"/>
       <c r="CO18" s="25"/>
       <c r="CP18" s="25"/>
+      <c r="CQ18" s="1"/>
+      <c r="CR18" s="1"/>
+      <c r="CS18" s="1"/>
+      <c r="CT18" s="1"/>
+      <c r="CU18" s="1"/>
     </row>
-    <row r="19" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>232</v>
       </c>
@@ -4771,7 +4926,7 @@
       <c r="H19" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J19" s="1"/>
@@ -4869,8 +5024,13 @@
         <v>252</v>
       </c>
       <c r="CP19" s="25"/>
+      <c r="CQ19" s="1"/>
+      <c r="CR19" s="1"/>
+      <c r="CS19" s="1"/>
+      <c r="CT19" s="1"/>
+      <c r="CU19" s="1"/>
     </row>
-    <row r="20" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>233</v>
       </c>
@@ -4895,7 +5055,7 @@
       <c r="H20" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J20" s="1"/>
@@ -4989,8 +5149,13 @@
         <v>252</v>
       </c>
       <c r="CP20" s="25"/>
+      <c r="CQ20" s="1"/>
+      <c r="CR20" s="1"/>
+      <c r="CS20" s="1"/>
+      <c r="CT20" s="1"/>
+      <c r="CU20" s="1"/>
     </row>
-    <row r="21" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>234</v>
       </c>
@@ -5015,7 +5180,7 @@
       <c r="H21" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I21" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J21" s="1"/>
@@ -5115,8 +5280,13 @@
         <v>252</v>
       </c>
       <c r="CP21" s="25"/>
+      <c r="CQ21" s="1"/>
+      <c r="CR21" s="1"/>
+      <c r="CS21" s="1"/>
+      <c r="CT21" s="1"/>
+      <c r="CU21" s="1"/>
     </row>
-    <row r="22" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>235</v>
       </c>
@@ -5141,7 +5311,7 @@
       <c r="H22" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I22" s="34" t="s">
+      <c r="I22" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J22" s="1"/>
@@ -5237,8 +5407,13 @@
         <v>252</v>
       </c>
       <c r="CP22" s="25"/>
+      <c r="CQ22" s="1"/>
+      <c r="CR22" s="1"/>
+      <c r="CS22" s="1"/>
+      <c r="CT22" s="1"/>
+      <c r="CU22" s="1"/>
     </row>
-    <row r="23" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>236</v>
       </c>
@@ -5263,7 +5438,7 @@
       <c r="H23" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I23" s="34" t="s">
+      <c r="I23" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J23" s="1"/>
@@ -5359,8 +5534,13 @@
         <v>252</v>
       </c>
       <c r="CP23" s="25"/>
+      <c r="CQ23" s="1"/>
+      <c r="CR23" s="1"/>
+      <c r="CS23" s="1"/>
+      <c r="CT23" s="1"/>
+      <c r="CU23" s="1"/>
     </row>
-    <row r="24" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>237</v>
       </c>
@@ -5385,7 +5565,7 @@
       <c r="H24" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J24" s="1"/>
@@ -5481,8 +5661,13 @@
         <v>252</v>
       </c>
       <c r="CP24" s="25"/>
+      <c r="CQ24" s="1"/>
+      <c r="CR24" s="1"/>
+      <c r="CS24" s="1"/>
+      <c r="CT24" s="1"/>
+      <c r="CU24" s="1"/>
     </row>
-    <row r="25" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>238</v>
       </c>
@@ -5507,7 +5692,7 @@
       <c r="H25" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="I25" s="34" t="s">
+      <c r="I25" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J25" s="1"/>
@@ -5601,8 +5786,13 @@
         <v>252</v>
       </c>
       <c r="CP25" s="25"/>
+      <c r="CQ25" s="1"/>
+      <c r="CR25" s="1"/>
+      <c r="CS25" s="1"/>
+      <c r="CT25" s="1"/>
+      <c r="CU25" s="1"/>
     </row>
-    <row r="26" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>239</v>
       </c>
@@ -5627,7 +5817,7 @@
       <c r="H26" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="I26" s="34" t="s">
+      <c r="I26" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J26" s="1"/>
@@ -5721,8 +5911,13 @@
         <v>252</v>
       </c>
       <c r="CP26" s="25"/>
+      <c r="CQ26" s="1"/>
+      <c r="CR26" s="1"/>
+      <c r="CS26" s="1"/>
+      <c r="CT26" s="1"/>
+      <c r="CU26" s="1"/>
     </row>
-    <row r="27" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>240</v>
       </c>
@@ -5747,7 +5942,7 @@
       <c r="H27" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J27" s="1"/>
@@ -5843,8 +6038,13 @@
         <v>252</v>
       </c>
       <c r="CP27" s="25"/>
+      <c r="CQ27" s="1"/>
+      <c r="CR27" s="1"/>
+      <c r="CS27" s="1"/>
+      <c r="CT27" s="1"/>
+      <c r="CU27" s="1"/>
     </row>
-    <row r="28" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>241</v>
       </c>
@@ -5869,7 +6069,7 @@
       <c r="H28" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J28" s="1"/>
@@ -5967,8 +6167,13 @@
         <v>252</v>
       </c>
       <c r="CP28" s="25"/>
+      <c r="CQ28" s="1"/>
+      <c r="CR28" s="1"/>
+      <c r="CS28" s="1"/>
+      <c r="CT28" s="1"/>
+      <c r="CU28" s="1"/>
     </row>
-    <row r="29" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>242</v>
       </c>
@@ -5993,7 +6198,7 @@
       <c r="H29" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="I29" s="34" t="s">
+      <c r="I29" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J29" s="1"/>
@@ -6091,8 +6296,13 @@
         <v>252</v>
       </c>
       <c r="CP29" s="25"/>
+      <c r="CQ29" s="1"/>
+      <c r="CR29" s="1"/>
+      <c r="CS29" s="1"/>
+      <c r="CT29" s="1"/>
+      <c r="CU29" s="1"/>
     </row>
-    <row r="30" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>243</v>
       </c>
@@ -6117,7 +6327,7 @@
       <c r="H30" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="I30" s="34" t="s">
+      <c r="I30" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J30" s="1"/>
@@ -6211,29 +6421,36 @@
         <v>252</v>
       </c>
       <c r="CP30" s="25"/>
+      <c r="CQ30" s="1"/>
+      <c r="CR30" s="1"/>
+      <c r="CS30" s="1"/>
+      <c r="CT30" s="1"/>
+      <c r="CU30" s="1"/>
     </row>
-    <row r="31" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>488</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>489</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>244</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="34"/>
+      <c r="I31" s="40" t="s">
+        <v>173</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -6319,8 +6536,13 @@
       <c r="CN31" s="1"/>
       <c r="CO31" s="1"/>
       <c r="CP31" s="25"/>
+      <c r="CQ31" s="1"/>
+      <c r="CR31" s="1"/>
+      <c r="CS31" s="1"/>
+      <c r="CT31" s="1"/>
+      <c r="CU31" s="1"/>
     </row>
-    <row r="32" spans="1:94" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>331</v>
       </c>
@@ -6337,15 +6559,15 @@
         <v>244</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="I32" s="34" t="s">
+      <c r="I32" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J32" s="1"/>
@@ -6392,7 +6614,7 @@
         <v>326</v>
       </c>
       <c r="AW32" s="32" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AX32" s="1"/>
       <c r="AY32" s="1" t="s">
@@ -6443,8 +6665,13 @@
         <v>252</v>
       </c>
       <c r="CP32" s="1"/>
+      <c r="CQ32" s="1"/>
+      <c r="CR32" s="1"/>
+      <c r="CS32" s="1"/>
+      <c r="CT32" s="1"/>
+      <c r="CU32" s="1"/>
     </row>
-    <row r="33" spans="1:94" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:99" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>333</v>
       </c>
@@ -6461,15 +6688,15 @@
         <v>244</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="I33" s="34" t="s">
+      <c r="I33" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J33" s="1"/>
@@ -6522,7 +6749,7 @@
       </c>
       <c r="AZ33" s="1"/>
       <c r="BA33" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="BB33" s="1"/>
       <c r="BC33" s="1"/>
@@ -6567,8 +6794,13 @@
         <v>252</v>
       </c>
       <c r="CP33" s="1"/>
+      <c r="CQ33" s="1"/>
+      <c r="CR33" s="1"/>
+      <c r="CS33" s="1"/>
+      <c r="CT33" s="1"/>
+      <c r="CU33" s="1"/>
     </row>
-    <row r="34" spans="1:94" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:99" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>335</v>
       </c>
@@ -6585,15 +6817,15 @@
         <v>244</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="33" t="s">
         <v>407</v>
       </c>
-      <c r="H34" s="35" t="s">
-        <v>408</v>
-      </c>
-      <c r="I34" s="34" t="s">
+      <c r="I34" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J34" s="1"/>
@@ -6633,7 +6865,7 @@
       <c r="AR34" s="1"/>
       <c r="AS34" s="1"/>
       <c r="AT34" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AU34" s="1"/>
       <c r="AV34" s="1"/>
@@ -6687,8 +6919,13 @@
         <v>252</v>
       </c>
       <c r="CP34" s="1"/>
+      <c r="CQ34" s="1"/>
+      <c r="CR34" s="1"/>
+      <c r="CS34" s="1"/>
+      <c r="CT34" s="1"/>
+      <c r="CU34" s="1"/>
     </row>
-    <row r="35" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>336</v>
       </c>
@@ -6705,15 +6942,15 @@
         <v>244</v>
       </c>
       <c r="F35" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="I35" s="34" t="s">
+      <c r="I35" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J35" s="1"/>
@@ -6753,7 +6990,7 @@
       <c r="AR35" s="1"/>
       <c r="AS35" s="1"/>
       <c r="AT35" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AU35" s="1"/>
       <c r="AV35" s="1"/>
@@ -6807,8 +7044,13 @@
         <v>252</v>
       </c>
       <c r="CP35" s="1"/>
+      <c r="CQ35" s="1"/>
+      <c r="CR35" s="1"/>
+      <c r="CS35" s="1"/>
+      <c r="CT35" s="1"/>
+      <c r="CU35" s="1"/>
     </row>
-    <row r="36" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>337</v>
       </c>
@@ -6825,15 +7067,15 @@
         <v>244</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="I36" s="34" t="s">
+      <c r="I36" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J36" s="1"/>
@@ -6873,7 +7115,7 @@
       <c r="AR36" s="1"/>
       <c r="AS36" s="1"/>
       <c r="AT36" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AU36" s="1"/>
       <c r="AV36" s="1"/>
@@ -6927,8 +7169,13 @@
         <v>252</v>
       </c>
       <c r="CP36" s="1"/>
+      <c r="CQ36" s="1"/>
+      <c r="CR36" s="1"/>
+      <c r="CS36" s="1"/>
+      <c r="CT36" s="1"/>
+      <c r="CU36" s="1"/>
     </row>
-    <row r="37" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>338</v>
       </c>
@@ -6945,15 +7192,15 @@
         <v>244</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="I37" s="34" t="s">
+      <c r="I37" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J37" s="1"/>
@@ -6993,7 +7240,7 @@
       <c r="AR37" s="1"/>
       <c r="AS37" s="1"/>
       <c r="AT37" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AU37" s="1"/>
       <c r="AV37" s="1"/>
@@ -7047,8 +7294,13 @@
         <v>252</v>
       </c>
       <c r="CP37" s="1"/>
+      <c r="CQ37" s="1"/>
+      <c r="CR37" s="1"/>
+      <c r="CS37" s="1"/>
+      <c r="CT37" s="1"/>
+      <c r="CU37" s="1"/>
     </row>
-    <row r="38" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>339</v>
       </c>
@@ -7065,15 +7317,15 @@
         <v>244</v>
       </c>
       <c r="F38" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="I38" s="34" t="s">
+      <c r="I38" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J38" s="1"/>
@@ -7113,7 +7365,7 @@
       <c r="AR38" s="1"/>
       <c r="AS38" s="1"/>
       <c r="AT38" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AU38" s="1"/>
       <c r="AV38" s="1"/>
@@ -7167,8 +7419,13 @@
         <v>252</v>
       </c>
       <c r="CP38" s="1"/>
+      <c r="CQ38" s="1"/>
+      <c r="CR38" s="1"/>
+      <c r="CS38" s="1"/>
+      <c r="CT38" s="1"/>
+      <c r="CU38" s="1"/>
     </row>
-    <row r="39" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>340</v>
       </c>
@@ -7185,15 +7442,15 @@
         <v>244</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="I39" s="34" t="s">
+      <c r="I39" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J39" s="1"/>
@@ -7233,7 +7490,7 @@
       <c r="AR39" s="1"/>
       <c r="AS39" s="1"/>
       <c r="AT39" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AU39" s="1"/>
       <c r="AV39" s="1"/>
@@ -7287,8 +7544,13 @@
         <v>252</v>
       </c>
       <c r="CP39" s="1"/>
+      <c r="CQ39" s="1"/>
+      <c r="CR39" s="1"/>
+      <c r="CS39" s="1"/>
+      <c r="CT39" s="1"/>
+      <c r="CU39" s="1"/>
     </row>
-    <row r="40" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>341</v>
       </c>
@@ -7305,15 +7567,15 @@
         <v>244</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="I40" s="34" t="s">
+      <c r="I40" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J40" s="1"/>
@@ -7353,7 +7615,7 @@
       <c r="AR40" s="1"/>
       <c r="AS40" s="1"/>
       <c r="AT40" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AU40" s="1"/>
       <c r="AV40" s="1"/>
@@ -7407,8 +7669,13 @@
         <v>252</v>
       </c>
       <c r="CP40" s="1"/>
+      <c r="CQ40" s="1"/>
+      <c r="CR40" s="1"/>
+      <c r="CS40" s="1"/>
+      <c r="CT40" s="1"/>
+      <c r="CU40" s="1"/>
     </row>
-    <row r="41" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>342</v>
       </c>
@@ -7425,15 +7692,15 @@
         <v>244</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="I41" s="34" t="s">
+      <c r="I41" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J41" s="1"/>
@@ -7473,7 +7740,7 @@
       <c r="AR41" s="1"/>
       <c r="AS41" s="1"/>
       <c r="AT41" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AU41" s="1"/>
       <c r="AV41" s="1"/>
@@ -7527,8 +7794,13 @@
         <v>252</v>
       </c>
       <c r="CP41" s="1"/>
+      <c r="CQ41" s="1"/>
+      <c r="CR41" s="1"/>
+      <c r="CS41" s="1"/>
+      <c r="CT41" s="1"/>
+      <c r="CU41" s="1"/>
     </row>
-    <row r="42" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>343</v>
       </c>
@@ -7545,13 +7817,13 @@
         <v>244</v>
       </c>
       <c r="F42" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>431</v>
-      </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="34" t="s">
+      <c r="I42" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J42" s="1"/>
@@ -7591,7 +7863,7 @@
       <c r="AR42" s="1"/>
       <c r="AS42" s="1"/>
       <c r="AT42" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AU42" s="1"/>
       <c r="AV42" s="1"/>
@@ -7645,8 +7917,13 @@
         <v>252</v>
       </c>
       <c r="CP42" s="1"/>
+      <c r="CQ42" s="1"/>
+      <c r="CR42" s="1"/>
+      <c r="CS42" s="1"/>
+      <c r="CT42" s="1"/>
+      <c r="CU42" s="1"/>
     </row>
-    <row r="43" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>344</v>
       </c>
@@ -7663,13 +7940,13 @@
         <v>244</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="G43" s="1" t="s">
-        <v>433</v>
-      </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="34" t="s">
+      <c r="I43" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J43" s="1"/>
@@ -7709,7 +7986,7 @@
       <c r="AR43" s="1"/>
       <c r="AS43" s="1"/>
       <c r="AT43" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AU43" s="1"/>
       <c r="AV43" s="1"/>
@@ -7763,8 +8040,13 @@
         <v>252</v>
       </c>
       <c r="CP43" s="1"/>
+      <c r="CQ43" s="1"/>
+      <c r="CR43" s="1"/>
+      <c r="CS43" s="1"/>
+      <c r="CT43" s="1"/>
+      <c r="CU43" s="1"/>
     </row>
-    <row r="44" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>345</v>
       </c>
@@ -7781,13 +8063,13 @@
         <v>244</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>435</v>
-      </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="34" t="s">
+      <c r="I44" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J44" s="1"/>
@@ -7827,7 +8109,7 @@
       <c r="AR44" s="1"/>
       <c r="AS44" s="1"/>
       <c r="AT44" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AU44" s="1"/>
       <c r="AV44" s="1"/>
@@ -7881,8 +8163,13 @@
         <v>252</v>
       </c>
       <c r="CP44" s="1"/>
+      <c r="CQ44" s="1"/>
+      <c r="CR44" s="1"/>
+      <c r="CS44" s="1"/>
+      <c r="CT44" s="1"/>
+      <c r="CU44" s="1"/>
     </row>
-    <row r="45" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>346</v>
       </c>
@@ -7899,13 +8186,13 @@
         <v>244</v>
       </c>
       <c r="F45" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>437</v>
-      </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="34" t="s">
+      <c r="I45" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J45" s="1"/>
@@ -7945,7 +8232,7 @@
       <c r="AR45" s="1"/>
       <c r="AS45" s="1"/>
       <c r="AT45" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AU45" s="1"/>
       <c r="AV45" s="1"/>
@@ -7999,8 +8286,13 @@
         <v>252</v>
       </c>
       <c r="CP45" s="1"/>
+      <c r="CQ45" s="1"/>
+      <c r="CR45" s="1"/>
+      <c r="CS45" s="1"/>
+      <c r="CT45" s="1"/>
+      <c r="CU45" s="1"/>
     </row>
-    <row r="46" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>347</v>
       </c>
@@ -8017,15 +8309,15 @@
         <v>244</v>
       </c>
       <c r="F46" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="I46" s="34" t="s">
+      <c r="I46" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J46" s="1"/>
@@ -8065,7 +8357,7 @@
       <c r="AR46" s="1"/>
       <c r="AS46" s="1"/>
       <c r="AT46" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AU46" s="1"/>
       <c r="AV46" s="1"/>
@@ -8119,8 +8411,13 @@
         <v>252</v>
       </c>
       <c r="CP46" s="1"/>
+      <c r="CQ46" s="1"/>
+      <c r="CR46" s="1"/>
+      <c r="CS46" s="1"/>
+      <c r="CT46" s="1"/>
+      <c r="CU46" s="1"/>
     </row>
-    <row r="47" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>348</v>
       </c>
@@ -8137,15 +8434,15 @@
         <v>244</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="I47" s="34" t="s">
+      <c r="I47" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J47" s="1"/>
@@ -8185,7 +8482,7 @@
       <c r="AR47" s="1"/>
       <c r="AS47" s="1"/>
       <c r="AT47" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AU47" s="1"/>
       <c r="AV47" s="1"/>
@@ -8239,8 +8536,13 @@
         <v>252</v>
       </c>
       <c r="CP47" s="1"/>
+      <c r="CQ47" s="1"/>
+      <c r="CR47" s="1"/>
+      <c r="CS47" s="1"/>
+      <c r="CT47" s="1"/>
+      <c r="CU47" s="1"/>
     </row>
-    <row r="48" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>349</v>
       </c>
@@ -8257,15 +8559,15 @@
         <v>244</v>
       </c>
       <c r="F48" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="I48" s="34" t="s">
+      <c r="I48" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J48" s="1"/>
@@ -8305,7 +8607,7 @@
       <c r="AR48" s="1"/>
       <c r="AS48" s="1"/>
       <c r="AT48" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AU48" s="1"/>
       <c r="AV48" s="1"/>
@@ -8359,8 +8661,13 @@
         <v>252</v>
       </c>
       <c r="CP48" s="1"/>
+      <c r="CQ48" s="1"/>
+      <c r="CR48" s="1"/>
+      <c r="CS48" s="1"/>
+      <c r="CT48" s="1"/>
+      <c r="CU48" s="1"/>
     </row>
-    <row r="49" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>350</v>
       </c>
@@ -8377,15 +8684,15 @@
         <v>244</v>
       </c>
       <c r="F49" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="I49" s="34" t="s">
+      <c r="I49" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J49" s="1"/>
@@ -8425,7 +8732,7 @@
       <c r="AR49" s="1"/>
       <c r="AS49" s="1"/>
       <c r="AT49" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AU49" s="1"/>
       <c r="AV49" s="1"/>
@@ -8479,8 +8786,13 @@
         <v>252</v>
       </c>
       <c r="CP49" s="1"/>
+      <c r="CQ49" s="1"/>
+      <c r="CR49" s="1"/>
+      <c r="CS49" s="1"/>
+      <c r="CT49" s="1"/>
+      <c r="CU49" s="1"/>
     </row>
-    <row r="50" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>351</v>
       </c>
@@ -8497,13 +8809,13 @@
         <v>244</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>451</v>
-      </c>
       <c r="H50" s="1"/>
-      <c r="I50" s="34" t="s">
+      <c r="I50" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J50" s="1"/>
@@ -8543,7 +8855,7 @@
       <c r="AR50" s="1"/>
       <c r="AS50" s="1"/>
       <c r="AT50" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AU50" s="1"/>
       <c r="AV50" s="1"/>
@@ -8597,8 +8909,13 @@
         <v>252</v>
       </c>
       <c r="CP50" s="1"/>
+      <c r="CQ50" s="1"/>
+      <c r="CR50" s="1"/>
+      <c r="CS50" s="1"/>
+      <c r="CT50" s="1"/>
+      <c r="CU50" s="1"/>
     </row>
-    <row r="51" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>352</v>
       </c>
@@ -8615,13 +8932,13 @@
         <v>244</v>
       </c>
       <c r="F51" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>453</v>
-      </c>
       <c r="H51" s="1"/>
-      <c r="I51" s="34" t="s">
+      <c r="I51" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J51" s="1"/>
@@ -8661,7 +8978,7 @@
       <c r="AR51" s="1"/>
       <c r="AS51" s="1"/>
       <c r="AT51" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AU51" s="1"/>
       <c r="AV51" s="1"/>
@@ -8715,8 +9032,13 @@
         <v>252</v>
       </c>
       <c r="CP51" s="1"/>
+      <c r="CQ51" s="1"/>
+      <c r="CR51" s="1"/>
+      <c r="CS51" s="1"/>
+      <c r="CT51" s="1"/>
+      <c r="CU51" s="1"/>
     </row>
-    <row r="52" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>353</v>
       </c>
@@ -8733,15 +9055,15 @@
         <v>244</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="I52" s="34" t="s">
+      <c r="I52" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J52" s="1"/>
@@ -8781,7 +9103,7 @@
       <c r="AR52" s="1"/>
       <c r="AS52" s="1"/>
       <c r="AT52" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AU52" s="1"/>
       <c r="AV52" s="1"/>
@@ -8835,8 +9157,13 @@
         <v>252</v>
       </c>
       <c r="CP52" s="1"/>
+      <c r="CQ52" s="1"/>
+      <c r="CR52" s="1"/>
+      <c r="CS52" s="1"/>
+      <c r="CT52" s="1"/>
+      <c r="CU52" s="1"/>
     </row>
-    <row r="53" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>354</v>
       </c>
@@ -8853,15 +9180,15 @@
         <v>244</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="I53" s="34" t="s">
+      <c r="I53" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J53" s="1"/>
@@ -8901,7 +9228,7 @@
       <c r="AR53" s="1"/>
       <c r="AS53" s="1"/>
       <c r="AT53" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AU53" s="1"/>
       <c r="AV53" s="1"/>
@@ -8955,8 +9282,13 @@
         <v>252</v>
       </c>
       <c r="CP53" s="1"/>
+      <c r="CQ53" s="1"/>
+      <c r="CR53" s="1"/>
+      <c r="CS53" s="1"/>
+      <c r="CT53" s="1"/>
+      <c r="CU53" s="1"/>
     </row>
-    <row r="54" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>355</v>
       </c>
@@ -8973,13 +9305,13 @@
         <v>244</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>461</v>
-      </c>
       <c r="H54" s="1"/>
-      <c r="I54" s="34" t="s">
+      <c r="I54" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J54" s="1"/>
@@ -9019,7 +9351,7 @@
       <c r="AR54" s="1"/>
       <c r="AS54" s="1"/>
       <c r="AT54" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AU54" s="1"/>
       <c r="AV54" s="1"/>
@@ -9075,8 +9407,13 @@
         <v>252</v>
       </c>
       <c r="CP54" s="1"/>
+      <c r="CQ54" s="1"/>
+      <c r="CR54" s="1"/>
+      <c r="CS54" s="1"/>
+      <c r="CT54" s="1"/>
+      <c r="CU54" s="1"/>
     </row>
-    <row r="55" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>356</v>
       </c>
@@ -9093,13 +9430,13 @@
         <v>244</v>
       </c>
       <c r="F55" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="G55" s="1" t="s">
-        <v>463</v>
-      </c>
       <c r="H55" s="1"/>
-      <c r="I55" s="34" t="s">
+      <c r="I55" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J55" s="1"/>
@@ -9139,7 +9476,7 @@
       <c r="AR55" s="1"/>
       <c r="AS55" s="1"/>
       <c r="AT55" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AU55" s="1"/>
       <c r="AV55" s="1"/>
@@ -9195,8 +9532,13 @@
         <v>252</v>
       </c>
       <c r="CP55" s="1"/>
+      <c r="CQ55" s="1"/>
+      <c r="CR55" s="1"/>
+      <c r="CS55" s="1"/>
+      <c r="CT55" s="1"/>
+      <c r="CU55" s="1"/>
     </row>
-    <row r="56" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>357</v>
       </c>
@@ -9213,15 +9555,15 @@
         <v>244</v>
       </c>
       <c r="F56" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="H56" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="I56" s="34" t="s">
+      <c r="I56" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J56" s="1"/>
@@ -9261,7 +9603,7 @@
       <c r="AR56" s="1"/>
       <c r="AS56" s="1"/>
       <c r="AT56" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AU56" s="1"/>
       <c r="AV56" s="1"/>
@@ -9317,8 +9659,13 @@
         <v>252</v>
       </c>
       <c r="CP56" s="1"/>
+      <c r="CQ56" s="1"/>
+      <c r="CR56" s="1"/>
+      <c r="CS56" s="1"/>
+      <c r="CT56" s="1"/>
+      <c r="CU56" s="1"/>
     </row>
-    <row r="57" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>358</v>
       </c>
@@ -9335,15 +9682,15 @@
         <v>244</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="G57" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="G57" s="1" t="s">
-        <v>468</v>
-      </c>
       <c r="H57" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="I57" s="34" t="s">
+        <v>465</v>
+      </c>
+      <c r="I57" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J57" s="1"/>
@@ -9383,7 +9730,7 @@
       <c r="AR57" s="1"/>
       <c r="AS57" s="1"/>
       <c r="AT57" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AU57" s="1"/>
       <c r="AV57" s="1"/>
@@ -9439,8 +9786,13 @@
         <v>252</v>
       </c>
       <c r="CP57" s="1"/>
+      <c r="CQ57" s="1"/>
+      <c r="CR57" s="1"/>
+      <c r="CS57" s="1"/>
+      <c r="CT57" s="1"/>
+      <c r="CU57" s="1"/>
     </row>
-    <row r="58" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>359</v>
       </c>
@@ -9457,15 +9809,15 @@
         <v>244</v>
       </c>
       <c r="F58" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="H58" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="I58" s="34" t="s">
+      <c r="I58" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J58" s="1"/>
@@ -9505,7 +9857,7 @@
       <c r="AR58" s="1"/>
       <c r="AS58" s="1"/>
       <c r="AT58" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AU58" s="1"/>
       <c r="AV58" s="1"/>
@@ -9561,8 +9913,13 @@
         <v>252</v>
       </c>
       <c r="CP58" s="1"/>
+      <c r="CQ58" s="1"/>
+      <c r="CR58" s="1"/>
+      <c r="CS58" s="1"/>
+      <c r="CT58" s="1"/>
+      <c r="CU58" s="1"/>
     </row>
-    <row r="59" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>360</v>
       </c>
@@ -9579,15 +9936,15 @@
         <v>244</v>
       </c>
       <c r="F59" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="G59" s="1" t="s">
-        <v>473</v>
-      </c>
       <c r="H59" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="I59" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="I59" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J59" s="1"/>
@@ -9627,7 +9984,7 @@
       <c r="AR59" s="1"/>
       <c r="AS59" s="1"/>
       <c r="AT59" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AU59" s="1"/>
       <c r="AV59" s="1"/>
@@ -9683,8 +10040,13 @@
         <v>252</v>
       </c>
       <c r="CP59" s="1"/>
+      <c r="CQ59" s="1"/>
+      <c r="CR59" s="1"/>
+      <c r="CS59" s="1"/>
+      <c r="CT59" s="1"/>
+      <c r="CU59" s="1"/>
     </row>
-    <row r="60" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>361</v>
       </c>
@@ -9701,15 +10063,15 @@
         <v>244</v>
       </c>
       <c r="F60" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="H60" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="I60" s="34" t="s">
+      <c r="I60" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J60" s="1"/>
@@ -9749,7 +10111,7 @@
       <c r="AR60" s="1"/>
       <c r="AS60" s="1"/>
       <c r="AT60" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AU60" s="1"/>
       <c r="AV60" s="1"/>
@@ -9760,7 +10122,7 @@
       </c>
       <c r="AZ60" s="1"/>
       <c r="BA60" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="BB60" s="1"/>
       <c r="BC60" s="1"/>
@@ -9805,8 +10167,13 @@
         <v>252</v>
       </c>
       <c r="CP60" s="1"/>
+      <c r="CQ60" s="1"/>
+      <c r="CR60" s="1"/>
+      <c r="CS60" s="1"/>
+      <c r="CT60" s="1"/>
+      <c r="CU60" s="1"/>
     </row>
-    <row r="61" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>362</v>
       </c>
@@ -9823,15 +10190,15 @@
         <v>244</v>
       </c>
       <c r="F61" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="H61" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="I61" s="34" t="s">
+      <c r="I61" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J61" s="1"/>
@@ -9871,7 +10238,7 @@
       <c r="AR61" s="1"/>
       <c r="AS61" s="1"/>
       <c r="AT61" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AU61" s="1"/>
       <c r="AV61" s="1"/>
@@ -9882,7 +10249,7 @@
       </c>
       <c r="AZ61" s="1"/>
       <c r="BA61" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="BB61" s="1"/>
       <c r="BC61" s="1"/>
@@ -9927,8 +10294,13 @@
         <v>252</v>
       </c>
       <c r="CP61" s="1"/>
+      <c r="CQ61" s="1"/>
+      <c r="CR61" s="1"/>
+      <c r="CS61" s="1"/>
+      <c r="CT61" s="1"/>
+      <c r="CU61" s="1"/>
     </row>
-    <row r="62" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>363</v>
       </c>
@@ -9945,15 +10317,15 @@
         <v>244</v>
       </c>
       <c r="F62" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="H62" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="I62" s="34" t="s">
+      <c r="I62" s="40" t="s">
         <v>173</v>
       </c>
       <c r="J62" s="1"/>
@@ -9993,7 +10365,7 @@
       <c r="AR62" s="1"/>
       <c r="AS62" s="1"/>
       <c r="AT62" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AU62" s="1"/>
       <c r="AV62" s="1"/>
@@ -10049,128 +10421,271 @@
         <v>252</v>
       </c>
       <c r="CP62" s="1"/>
+      <c r="CQ62" s="1"/>
+      <c r="CR62" s="1"/>
+      <c r="CS62" s="1"/>
+      <c r="CT62" s="1"/>
+      <c r="CU62" s="1"/>
     </row>
-    <row r="63" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A63" s="37" t="s">
         <v>364</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="37" t="s">
+        <v>482</v>
+      </c>
+      <c r="G63" s="37" t="s">
         <v>483</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="H63" s="37" t="s">
         <v>484</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="I63" s="34" t="s">
+      <c r="I63" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1"/>
-      <c r="V63" s="1"/>
-      <c r="W63" s="1"/>
-      <c r="X63" s="1"/>
-      <c r="Y63" s="1"/>
-      <c r="Z63" s="1"/>
-      <c r="AA63" s="1"/>
-      <c r="AB63" s="1"/>
-      <c r="AC63" s="1"/>
-      <c r="AD63" s="1"/>
-      <c r="AE63" s="1"/>
-      <c r="AF63" s="1"/>
-      <c r="AG63" s="1"/>
-      <c r="AH63" s="1"/>
-      <c r="AI63" s="1"/>
-      <c r="AJ63" s="1"/>
-      <c r="AK63" s="1"/>
-      <c r="AL63" s="1"/>
-      <c r="AM63" s="1"/>
-      <c r="AN63" s="1"/>
-      <c r="AO63" s="1"/>
-      <c r="AP63" s="1"/>
-      <c r="AQ63" s="1"/>
-      <c r="AR63" s="1"/>
-      <c r="AS63" s="1"/>
-      <c r="AT63" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="AU63" s="1"/>
-      <c r="AV63" s="1"/>
-      <c r="AW63" s="32"/>
-      <c r="AX63" s="1"/>
-      <c r="AY63" s="1" t="s">
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
+      <c r="O63" s="37"/>
+      <c r="P63" s="37"/>
+      <c r="Q63" s="37"/>
+      <c r="R63" s="37"/>
+      <c r="S63" s="37"/>
+      <c r="T63" s="37"/>
+      <c r="U63" s="37"/>
+      <c r="V63" s="37"/>
+      <c r="W63" s="37"/>
+      <c r="X63" s="37"/>
+      <c r="Y63" s="37"/>
+      <c r="Z63" s="37"/>
+      <c r="AA63" s="37"/>
+      <c r="AB63" s="37"/>
+      <c r="AC63" s="37"/>
+      <c r="AD63" s="37"/>
+      <c r="AE63" s="37"/>
+      <c r="AF63" s="37"/>
+      <c r="AG63" s="37"/>
+      <c r="AH63" s="37"/>
+      <c r="AI63" s="37"/>
+      <c r="AJ63" s="37"/>
+      <c r="AK63" s="37"/>
+      <c r="AL63" s="37"/>
+      <c r="AM63" s="37"/>
+      <c r="AN63" s="37"/>
+      <c r="AO63" s="37"/>
+      <c r="AP63" s="37"/>
+      <c r="AQ63" s="37"/>
+      <c r="AR63" s="37"/>
+      <c r="AS63" s="37"/>
+      <c r="AT63" s="37" t="s">
+        <v>396</v>
+      </c>
+      <c r="AU63" s="37"/>
+      <c r="AV63" s="37"/>
+      <c r="AW63" s="38"/>
+      <c r="AX63" s="37"/>
+      <c r="AY63" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="AZ63" s="1"/>
-      <c r="BA63" s="1">
+      <c r="AZ63" s="37"/>
+      <c r="BA63" s="37">
         <v>28</v>
       </c>
-      <c r="BB63" s="1"/>
-      <c r="BC63" s="1"/>
-      <c r="BD63" s="1"/>
-      <c r="BE63" s="1"/>
-      <c r="BF63" s="1"/>
-      <c r="BG63" s="1"/>
-      <c r="BH63" s="1"/>
-      <c r="BI63" s="1"/>
-      <c r="BJ63" s="1"/>
-      <c r="BK63" s="1"/>
-      <c r="BL63" s="1"/>
-      <c r="BM63" s="1"/>
-      <c r="BN63" s="1"/>
-      <c r="BO63" s="1"/>
-      <c r="BP63" s="1"/>
-      <c r="BQ63" s="1"/>
-      <c r="BR63" s="1"/>
-      <c r="BS63" s="1"/>
-      <c r="BT63" s="1"/>
-      <c r="BU63" s="1"/>
-      <c r="BV63" s="1"/>
-      <c r="BW63" s="1"/>
-      <c r="BX63" s="1"/>
-      <c r="BY63" s="1"/>
-      <c r="BZ63" s="1"/>
-      <c r="CA63" s="1"/>
-      <c r="CB63" s="1"/>
-      <c r="CC63" s="1"/>
-      <c r="CD63" s="1"/>
-      <c r="CE63" s="1"/>
-      <c r="CF63" s="1"/>
-      <c r="CG63" s="1"/>
-      <c r="CH63" s="1"/>
-      <c r="CI63" s="1"/>
-      <c r="CJ63" s="1"/>
-      <c r="CK63" s="1"/>
-      <c r="CL63" s="1"/>
-      <c r="CM63" s="1"/>
-      <c r="CN63" s="1"/>
-      <c r="CO63" s="1" t="s">
+      <c r="BB63" s="37"/>
+      <c r="BC63" s="37"/>
+      <c r="BD63" s="37"/>
+      <c r="BE63" s="37"/>
+      <c r="BF63" s="37"/>
+      <c r="BG63" s="37"/>
+      <c r="BH63" s="37"/>
+      <c r="BI63" s="37"/>
+      <c r="BJ63" s="37"/>
+      <c r="BK63" s="37"/>
+      <c r="BL63" s="37"/>
+      <c r="BM63" s="37"/>
+      <c r="BN63" s="37"/>
+      <c r="BO63" s="37"/>
+      <c r="BP63" s="37"/>
+      <c r="BQ63" s="37"/>
+      <c r="BR63" s="37"/>
+      <c r="BS63" s="37"/>
+      <c r="BT63" s="37"/>
+      <c r="BU63" s="37"/>
+      <c r="BV63" s="37"/>
+      <c r="BW63" s="37"/>
+      <c r="BX63" s="37"/>
+      <c r="BY63" s="37"/>
+      <c r="BZ63" s="37"/>
+      <c r="CA63" s="37"/>
+      <c r="CB63" s="37"/>
+      <c r="CC63" s="37"/>
+      <c r="CD63" s="37"/>
+      <c r="CE63" s="37"/>
+      <c r="CF63" s="37"/>
+      <c r="CG63" s="37"/>
+      <c r="CH63" s="37"/>
+      <c r="CI63" s="37"/>
+      <c r="CJ63" s="37"/>
+      <c r="CK63" s="37"/>
+      <c r="CL63" s="37"/>
+      <c r="CM63" s="37"/>
+      <c r="CN63" s="37"/>
+      <c r="CO63" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="CP63" s="1"/>
+      <c r="CP63" s="37"/>
+      <c r="CQ63" s="37"/>
+      <c r="CR63" s="37"/>
+      <c r="CS63" s="37"/>
+      <c r="CT63" s="37"/>
+      <c r="CU63" s="37"/>
+    </row>
+    <row r="64" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B64" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="1"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="X64" s="1"/>
+      <c r="Y64" s="1"/>
+      <c r="Z64" s="1"/>
+      <c r="AA64" s="1"/>
+      <c r="AB64" s="1"/>
+      <c r="AC64" s="1"/>
+      <c r="AD64" s="1"/>
+      <c r="AE64" s="1"/>
+      <c r="AF64" s="1"/>
+      <c r="AG64" s="1"/>
+      <c r="AH64" s="1"/>
+      <c r="AI64" s="1"/>
+      <c r="AJ64" s="1"/>
+      <c r="AK64" s="1"/>
+      <c r="AL64" s="1"/>
+      <c r="AM64" s="1"/>
+      <c r="AN64" s="1"/>
+      <c r="AO64" s="1"/>
+      <c r="AP64" s="1"/>
+      <c r="AQ64" s="1"/>
+      <c r="AR64" s="1"/>
+      <c r="AS64" s="1"/>
+      <c r="AT64" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="AU64" s="1"/>
+      <c r="AV64" s="1"/>
+      <c r="AW64" s="1"/>
+      <c r="AX64" s="1"/>
+      <c r="AY64" s="1"/>
+      <c r="AZ64" s="1"/>
+      <c r="BA64" s="1"/>
+      <c r="BB64" s="1"/>
+      <c r="BC64" s="1"/>
+      <c r="BD64" s="1"/>
+      <c r="BE64" s="1"/>
+      <c r="BF64" s="1"/>
+      <c r="BG64" s="1"/>
+      <c r="BH64" s="1"/>
+      <c r="BI64" s="1"/>
+      <c r="BJ64" s="1"/>
+      <c r="BK64" s="1"/>
+      <c r="BL64" s="1"/>
+      <c r="BM64" s="1"/>
+      <c r="BN64" s="1"/>
+      <c r="BO64" s="1"/>
+      <c r="BP64" s="1"/>
+      <c r="BQ64" s="1"/>
+      <c r="BR64" s="1"/>
+      <c r="BS64" s="1"/>
+      <c r="BT64" s="1"/>
+      <c r="BU64" s="1"/>
+      <c r="BV64" s="1"/>
+      <c r="BW64" s="1"/>
+      <c r="BX64" s="1"/>
+      <c r="BY64" s="1"/>
+      <c r="BZ64" s="1"/>
+      <c r="CA64" s="1"/>
+      <c r="CB64" s="1"/>
+      <c r="CC64" s="1"/>
+      <c r="CD64" s="1"/>
+      <c r="CE64" s="1"/>
+      <c r="CF64" s="1"/>
+      <c r="CG64" s="1"/>
+      <c r="CH64" s="1"/>
+      <c r="CI64" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="CJ64" s="1"/>
+      <c r="CK64" s="1"/>
+      <c r="CL64" s="1"/>
+      <c r="CM64" s="1"/>
+      <c r="CN64" s="1"/>
+      <c r="CO64" s="1"/>
+      <c r="CP64" s="1"/>
+      <c r="CQ64" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="CR64" s="35" t="s">
+        <v>497</v>
+      </c>
+      <c r="CS64" s="34" t="s">
+        <v>493</v>
+      </c>
+      <c r="CT64" s="36" t="s">
+        <v>498</v>
+      </c>
+      <c r="CU64" s="1" t="s">
+        <v>499</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Types of Login Scenarios
</commit_message>
<xml_diff>
--- a/Engage/Research-Smoke/src/main/resources/excelfiles/Research_Smoke.xlsx
+++ b/Engage/Research-Smoke/src/main/resources/excelfiles/Research_Smoke.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0251F812-222D-48D3-B896-0197E953FCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="598" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="598" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="516">
   <si>
     <t>Environment</t>
   </si>
@@ -1663,8 +1662,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1726,8 +1726,19 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1774,6 +1785,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -1854,7 +1895,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1904,15 +1945,19 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Hyperlink 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="4"/>
+    <cellStyle name="Hyperlink 2 2" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="5"/>
+    <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2189,7 +2234,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2199,8 +2244,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2231,7 +2276,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2240,9 +2285,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2269,14 +2314,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -2286,10 +2331,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2407,44 +2452,44 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CU65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C65"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="40.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="66" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="40.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="66.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:99">
@@ -2769,7 +2814,7 @@
       <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J2" s="4"/>
@@ -2888,7 +2933,7 @@
       <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="44" t="s">
+      <c r="I3" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -3087,7 +3132,7 @@
       <c r="H4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I4" s="44" t="s">
+      <c r="I4" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J4" s="11" t="s">
@@ -3220,7 +3265,7 @@
       <c r="H5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J5" s="11"/>
@@ -3351,7 +3396,7 @@
       <c r="H6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I6" s="44" t="s">
+      <c r="I6" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J6" s="11"/>
@@ -3472,7 +3517,7 @@
       <c r="H7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J7" s="11" t="s">
@@ -3597,7 +3642,7 @@
       <c r="H8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="44" t="s">
+      <c r="I8" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J8" s="11"/>
@@ -3718,7 +3763,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="44" t="s">
+      <c r="I9" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J9" s="1"/>
@@ -3849,7 +3894,7 @@
         <v>190</v>
       </c>
       <c r="H10" s="17"/>
-      <c r="I10" s="44" t="s">
+      <c r="I10" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -3980,7 +4025,7 @@
         <v>194</v>
       </c>
       <c r="H11" s="17"/>
-      <c r="I11" s="44" t="s">
+      <c r="I11" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J11" s="18" t="s">
@@ -4107,7 +4152,7 @@
         <v>198</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="45" t="s">
         <v>503</v>
       </c>
       <c r="J12" s="18" t="s">
@@ -4234,7 +4279,7 @@
         <v>202</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="44" t="s">
+      <c r="I13" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J13" s="18" t="s">
@@ -4361,7 +4406,7 @@
         <v>206</v>
       </c>
       <c r="H14" s="21"/>
-      <c r="I14" s="44" t="s">
+      <c r="I14" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J14" s="22" t="s">
@@ -4488,7 +4533,7 @@
       <c r="H15" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="44" t="s">
+      <c r="I15" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J15" s="11" t="s">
@@ -4619,7 +4664,7 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="44" t="s">
+      <c r="I16" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J16" s="11"/>
@@ -4740,7 +4785,7 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="44" t="s">
+      <c r="I17" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J17" s="11"/>
@@ -4863,7 +4908,7 @@
         <v>273</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="44" t="s">
+      <c r="I18" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J18" s="26"/>
@@ -4992,7 +5037,7 @@
       <c r="H19" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I19" s="44" t="s">
+      <c r="I19" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J19" s="1"/>
@@ -5121,7 +5166,7 @@
       <c r="H20" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I20" s="44" t="s">
+      <c r="I20" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J20" s="1"/>
@@ -5246,7 +5291,7 @@
       <c r="H21" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I21" s="44" t="s">
+      <c r="I21" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J21" s="1"/>
@@ -5377,7 +5422,7 @@
       <c r="H22" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I22" s="44" t="s">
+      <c r="I22" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J22" s="1"/>
@@ -5504,7 +5549,7 @@
       <c r="H23" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I23" s="44" t="s">
+      <c r="I23" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J23" s="1"/>
@@ -5631,7 +5676,7 @@
       <c r="H24" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I24" s="44" t="s">
+      <c r="I24" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J24" s="1"/>
@@ -5758,7 +5803,7 @@
       <c r="H25" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="I25" s="44" t="s">
+      <c r="I25" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J25" s="1"/>
@@ -5883,7 +5928,7 @@
       <c r="H26" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="I26" s="44" t="s">
+      <c r="I26" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J26" s="1"/>
@@ -6008,7 +6053,7 @@
       <c r="H27" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I27" s="44" t="s">
+      <c r="I27" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J27" s="1"/>
@@ -6135,7 +6180,7 @@
       <c r="H28" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="I28" s="44" t="s">
+      <c r="I28" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J28" s="1"/>
@@ -6264,7 +6309,7 @@
       <c r="H29" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="I29" s="44" t="s">
+      <c r="I29" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J29" s="1"/>
@@ -6393,7 +6438,7 @@
       <c r="H30" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I30" s="44" t="s">
+      <c r="I30" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J30" s="1"/>
@@ -6514,7 +6559,7 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="44" t="s">
+      <c r="I31" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J31" s="1"/>
@@ -6633,7 +6678,7 @@
       <c r="H32" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="I32" s="44" t="s">
+      <c r="I32" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J32" s="1"/>
@@ -6762,7 +6807,7 @@
       <c r="H33" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="I33" s="44" t="s">
+      <c r="I33" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J33" s="1"/>
@@ -6891,7 +6936,7 @@
       <c r="H34" s="33" t="s">
         <v>406</v>
       </c>
-      <c r="I34" s="44" t="s">
+      <c r="I34" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J34" s="1"/>
@@ -7016,7 +7061,7 @@
       <c r="H35" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="I35" s="44" t="s">
+      <c r="I35" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J35" s="1"/>
@@ -7141,7 +7186,7 @@
       <c r="H36" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="I36" s="44" t="s">
+      <c r="I36" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J36" s="1"/>
@@ -7266,7 +7311,7 @@
       <c r="H37" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="I37" s="44" t="s">
+      <c r="I37" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J37" s="1"/>
@@ -7391,7 +7436,7 @@
       <c r="H38" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I38" s="44" t="s">
+      <c r="I38" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J38" s="1"/>
@@ -7516,7 +7561,7 @@
       <c r="H39" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="I39" s="44" t="s">
+      <c r="I39" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J39" s="1"/>
@@ -7641,7 +7686,7 @@
       <c r="H40" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="I40" s="44" t="s">
+      <c r="I40" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J40" s="1"/>
@@ -7766,7 +7811,7 @@
       <c r="H41" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="I41" s="44" t="s">
+      <c r="I41" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J41" s="1"/>
@@ -7889,7 +7934,7 @@
         <v>429</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="44" t="s">
+      <c r="I42" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J42" s="1"/>
@@ -8012,7 +8057,7 @@
         <v>431</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="44" t="s">
+      <c r="I43" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J43" s="1"/>
@@ -8135,7 +8180,7 @@
         <v>433</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="44" t="s">
+      <c r="I44" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J44" s="1"/>
@@ -8258,7 +8303,7 @@
         <v>435</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="44" t="s">
+      <c r="I45" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J45" s="1"/>
@@ -8383,7 +8428,7 @@
       <c r="H46" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="I46" s="44" t="s">
+      <c r="I46" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J46" s="1"/>
@@ -8508,7 +8553,7 @@
       <c r="H47" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="I47" s="44" t="s">
+      <c r="I47" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J47" s="1"/>
@@ -8633,7 +8678,7 @@
       <c r="H48" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="I48" s="44" t="s">
+      <c r="I48" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J48" s="1"/>
@@ -8758,7 +8803,7 @@
       <c r="H49" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I49" s="44" t="s">
+      <c r="I49" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J49" s="1"/>
@@ -8881,7 +8926,7 @@
         <v>449</v>
       </c>
       <c r="H50" s="1"/>
-      <c r="I50" s="44" t="s">
+      <c r="I50" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J50" s="1"/>
@@ -9004,7 +9049,7 @@
         <v>451</v>
       </c>
       <c r="H51" s="1"/>
-      <c r="I51" s="44" t="s">
+      <c r="I51" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J51" s="1"/>
@@ -9129,7 +9174,7 @@
       <c r="H52" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="I52" s="44" t="s">
+      <c r="I52" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J52" s="1"/>
@@ -9254,7 +9299,7 @@
       <c r="H53" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="I53" s="44" t="s">
+      <c r="I53" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J53" s="1"/>
@@ -9377,7 +9422,7 @@
         <v>459</v>
       </c>
       <c r="H54" s="1"/>
-      <c r="I54" s="44" t="s">
+      <c r="I54" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J54" s="1"/>
@@ -9502,7 +9547,7 @@
         <v>461</v>
       </c>
       <c r="H55" s="1"/>
-      <c r="I55" s="44" t="s">
+      <c r="I55" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J55" s="1"/>
@@ -9629,7 +9674,7 @@
       <c r="H56" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="I56" s="44" t="s">
+      <c r="I56" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J56" s="1"/>
@@ -9756,7 +9801,7 @@
       <c r="H57" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="I57" s="44" t="s">
+      <c r="I57" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J57" s="1"/>
@@ -9883,7 +9928,7 @@
       <c r="H58" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I58" s="44" t="s">
+      <c r="I58" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J58" s="1"/>
@@ -10010,7 +10055,7 @@
       <c r="H59" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I59" s="44" t="s">
+      <c r="I59" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J59" s="1"/>
@@ -10137,7 +10182,7 @@
       <c r="H60" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="I60" s="44" t="s">
+      <c r="I60" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J60" s="1"/>
@@ -10264,7 +10309,7 @@
       <c r="H61" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="I61" s="44" t="s">
+      <c r="I61" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J61" s="1"/>
@@ -10391,7 +10436,7 @@
       <c r="H62" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="I62" s="44" t="s">
+      <c r="I62" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J62" s="1"/>
@@ -10518,7 +10563,7 @@
       <c r="H63" s="37" t="s">
         <v>483</v>
       </c>
-      <c r="I63" s="44" t="s">
+      <c r="I63" s="47" t="s">
         <v>172</v>
       </c>
       <c r="J63" s="37"/>
@@ -10625,7 +10670,7 @@
         <v>487</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>515</v>
@@ -10643,8 +10688,8 @@
         <v>489</v>
       </c>
       <c r="H64" s="1"/>
-      <c r="I64" s="39" t="s">
-        <v>172</v>
+      <c r="I64" s="45" t="s">
+        <v>503</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
@@ -10893,9 +10938,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="W10" r:id="rId2" display="aansari1@zarca.com" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="W11:W14" r:id="rId3" display="aansari1@zarca.com" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com"/>
+    <hyperlink ref="W10" r:id="rId2" display="aansari1@zarca.com"/>
+    <hyperlink ref="W11:W14" r:id="rId3" display="aansari1@zarca.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>

</xml_diff>

<commit_message>
Updated Login Scenarios on all three servers
</commit_message>
<xml_diff>
--- a/Engage/Research-Smoke/src/main/resources/excelfiles/Research_Smoke.xlsx
+++ b/Engage/Research-Smoke/src/main/resources/excelfiles/Research_Smoke.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="521">
   <si>
     <t>Environment</t>
   </si>
@@ -1658,13 +1658,28 @@
   <si>
     <t>Gaurav</t>
   </si>
+  <si>
+    <t>Smoke_TC77</t>
+  </si>
+  <si>
+    <t>Smoke_TC78</t>
+  </si>
+  <si>
+    <t>Sajid</t>
+  </si>
+  <si>
+    <t>Invalid Credentials</t>
+  </si>
+  <si>
+    <t>Valid Credentials</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="12">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1737,8 +1752,52 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1785,6 +1844,131 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -1895,7 +2079,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1944,11 +2128,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="4" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2464,10 +2670,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CU65"/>
+  <dimension ref="A1:CU67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2814,7 +3020,7 @@
       <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J2" s="4"/>
@@ -2933,7 +3139,7 @@
       <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -3132,7 +3338,7 @@
       <c r="H4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J4" s="11" t="s">
@@ -3265,7 +3471,7 @@
       <c r="H5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J5" s="11"/>
@@ -3396,7 +3602,7 @@
       <c r="H6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J6" s="11"/>
@@ -3517,7 +3723,7 @@
       <c r="H7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J7" s="11" t="s">
@@ -3642,7 +3848,7 @@
       <c r="H8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="47" t="s">
+      <c r="I8" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J8" s="11"/>
@@ -3763,7 +3969,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="47" t="s">
+      <c r="I9" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J9" s="1"/>
@@ -3894,7 +4100,7 @@
         <v>190</v>
       </c>
       <c r="H10" s="17"/>
-      <c r="I10" s="47" t="s">
+      <c r="I10" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -4025,7 +4231,7 @@
         <v>194</v>
       </c>
       <c r="H11" s="17"/>
-      <c r="I11" s="47" t="s">
+      <c r="I11" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J11" s="18" t="s">
@@ -4134,7 +4340,7 @@
         <v>196</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>515</v>
@@ -4152,8 +4358,8 @@
         <v>198</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="45" t="s">
-        <v>503</v>
+      <c r="I12" s="69" t="s">
+        <v>172</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>317</v>
@@ -4279,7 +4485,7 @@
         <v>202</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="47" t="s">
+      <c r="I13" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J13" s="18" t="s">
@@ -4406,7 +4612,7 @@
         <v>206</v>
       </c>
       <c r="H14" s="21"/>
-      <c r="I14" s="47" t="s">
+      <c r="I14" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J14" s="22" t="s">
@@ -4533,7 +4739,7 @@
       <c r="H15" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I15" s="47" t="s">
+      <c r="I15" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J15" s="11" t="s">
@@ -4664,7 +4870,7 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="47" t="s">
+      <c r="I16" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J16" s="11"/>
@@ -4785,7 +4991,7 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="47" t="s">
+      <c r="I17" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J17" s="11"/>
@@ -4908,7 +5114,7 @@
         <v>273</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="47" t="s">
+      <c r="I18" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J18" s="26"/>
@@ -5037,7 +5243,7 @@
       <c r="H19" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I19" s="47" t="s">
+      <c r="I19" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J19" s="1"/>
@@ -5166,7 +5372,7 @@
       <c r="H20" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I20" s="47" t="s">
+      <c r="I20" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J20" s="1"/>
@@ -5291,7 +5497,7 @@
       <c r="H21" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I21" s="47" t="s">
+      <c r="I21" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J21" s="1"/>
@@ -5422,7 +5628,7 @@
       <c r="H22" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I22" s="47" t="s">
+      <c r="I22" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J22" s="1"/>
@@ -5549,7 +5755,7 @@
       <c r="H23" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I23" s="47" t="s">
+      <c r="I23" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J23" s="1"/>
@@ -5676,7 +5882,7 @@
       <c r="H24" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I24" s="47" t="s">
+      <c r="I24" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J24" s="1"/>
@@ -5803,7 +6009,7 @@
       <c r="H25" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="I25" s="47" t="s">
+      <c r="I25" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J25" s="1"/>
@@ -5928,7 +6134,7 @@
       <c r="H26" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="I26" s="47" t="s">
+      <c r="I26" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J26" s="1"/>
@@ -6053,7 +6259,7 @@
       <c r="H27" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I27" s="47" t="s">
+      <c r="I27" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J27" s="1"/>
@@ -6180,7 +6386,7 @@
       <c r="H28" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="I28" s="47" t="s">
+      <c r="I28" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J28" s="1"/>
@@ -6309,7 +6515,7 @@
       <c r="H29" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="I29" s="47" t="s">
+      <c r="I29" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J29" s="1"/>
@@ -6438,7 +6644,7 @@
       <c r="H30" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="I30" s="47" t="s">
+      <c r="I30" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J30" s="1"/>
@@ -6559,7 +6765,7 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="47" t="s">
+      <c r="I31" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J31" s="1"/>
@@ -6678,7 +6884,7 @@
       <c r="H32" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="I32" s="47" t="s">
+      <c r="I32" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J32" s="1"/>
@@ -6807,7 +7013,7 @@
       <c r="H33" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="I33" s="47" t="s">
+      <c r="I33" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J33" s="1"/>
@@ -6936,7 +7142,7 @@
       <c r="H34" s="33" t="s">
         <v>406</v>
       </c>
-      <c r="I34" s="47" t="s">
+      <c r="I34" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J34" s="1"/>
@@ -7061,7 +7267,7 @@
       <c r="H35" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="I35" s="47" t="s">
+      <c r="I35" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J35" s="1"/>
@@ -7186,7 +7392,7 @@
       <c r="H36" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="I36" s="47" t="s">
+      <c r="I36" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J36" s="1"/>
@@ -7311,7 +7517,7 @@
       <c r="H37" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="I37" s="47" t="s">
+      <c r="I37" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J37" s="1"/>
@@ -7436,7 +7642,7 @@
       <c r="H38" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I38" s="47" t="s">
+      <c r="I38" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J38" s="1"/>
@@ -7561,7 +7767,7 @@
       <c r="H39" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="I39" s="47" t="s">
+      <c r="I39" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J39" s="1"/>
@@ -7686,7 +7892,7 @@
       <c r="H40" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="I40" s="47" t="s">
+      <c r="I40" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J40" s="1"/>
@@ -7811,7 +8017,7 @@
       <c r="H41" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="I41" s="47" t="s">
+      <c r="I41" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J41" s="1"/>
@@ -7934,7 +8140,7 @@
         <v>429</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="47" t="s">
+      <c r="I42" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J42" s="1"/>
@@ -8057,7 +8263,7 @@
         <v>431</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="47" t="s">
+      <c r="I43" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J43" s="1"/>
@@ -8180,7 +8386,7 @@
         <v>433</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="47" t="s">
+      <c r="I44" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J44" s="1"/>
@@ -8303,7 +8509,7 @@
         <v>435</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="47" t="s">
+      <c r="I45" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J45" s="1"/>
@@ -8428,7 +8634,7 @@
       <c r="H46" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="I46" s="47" t="s">
+      <c r="I46" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J46" s="1"/>
@@ -8553,7 +8759,7 @@
       <c r="H47" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="I47" s="47" t="s">
+      <c r="I47" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J47" s="1"/>
@@ -8678,7 +8884,7 @@
       <c r="H48" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="I48" s="47" t="s">
+      <c r="I48" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J48" s="1"/>
@@ -8803,7 +9009,7 @@
       <c r="H49" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I49" s="47" t="s">
+      <c r="I49" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J49" s="1"/>
@@ -8926,7 +9132,7 @@
         <v>449</v>
       </c>
       <c r="H50" s="1"/>
-      <c r="I50" s="47" t="s">
+      <c r="I50" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J50" s="1"/>
@@ -9049,7 +9255,7 @@
         <v>451</v>
       </c>
       <c r="H51" s="1"/>
-      <c r="I51" s="47" t="s">
+      <c r="I51" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J51" s="1"/>
@@ -9174,7 +9380,7 @@
       <c r="H52" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="I52" s="47" t="s">
+      <c r="I52" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J52" s="1"/>
@@ -9299,7 +9505,7 @@
       <c r="H53" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="I53" s="47" t="s">
+      <c r="I53" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J53" s="1"/>
@@ -9422,7 +9628,7 @@
         <v>459</v>
       </c>
       <c r="H54" s="1"/>
-      <c r="I54" s="47" t="s">
+      <c r="I54" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J54" s="1"/>
@@ -9547,7 +9753,7 @@
         <v>461</v>
       </c>
       <c r="H55" s="1"/>
-      <c r="I55" s="47" t="s">
+      <c r="I55" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J55" s="1"/>
@@ -9674,7 +9880,7 @@
       <c r="H56" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="I56" s="47" t="s">
+      <c r="I56" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J56" s="1"/>
@@ -9801,7 +10007,7 @@
       <c r="H57" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="I57" s="47" t="s">
+      <c r="I57" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J57" s="1"/>
@@ -9928,7 +10134,7 @@
       <c r="H58" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I58" s="47" t="s">
+      <c r="I58" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J58" s="1"/>
@@ -10055,7 +10261,7 @@
       <c r="H59" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I59" s="47" t="s">
+      <c r="I59" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J59" s="1"/>
@@ -10182,7 +10388,7 @@
       <c r="H60" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="I60" s="47" t="s">
+      <c r="I60" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J60" s="1"/>
@@ -10309,7 +10515,7 @@
       <c r="H61" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="I61" s="47" t="s">
+      <c r="I61" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J61" s="1"/>
@@ -10436,7 +10642,7 @@
       <c r="H62" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="I62" s="47" t="s">
+      <c r="I62" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J62" s="1"/>
@@ -10563,7 +10769,7 @@
       <c r="H63" s="37" t="s">
         <v>483</v>
       </c>
-      <c r="I63" s="47" t="s">
+      <c r="I63" s="69" t="s">
         <v>172</v>
       </c>
       <c r="J63" s="37"/>
@@ -10670,7 +10876,7 @@
         <v>487</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>515</v>
@@ -10688,8 +10894,8 @@
         <v>489</v>
       </c>
       <c r="H64" s="1"/>
-      <c r="I64" s="45" t="s">
-        <v>503</v>
+      <c r="I64" s="69" t="s">
+        <v>172</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
@@ -10801,139 +11007,369 @@
       </c>
     </row>
     <row r="65" spans="1:99">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="37" t="s">
         <v>504</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="37" t="s">
         <v>515</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="37" t="s">
         <v>505</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" s="37" t="s">
         <v>506</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" s="37" t="s">
         <v>507</v>
       </c>
-      <c r="G65" s="1" t="s">
+      <c r="G65" s="37" t="s">
         <v>508</v>
       </c>
-      <c r="H65" s="1" t="s">
+      <c r="H65" s="37" t="s">
         <v>509</v>
       </c>
       <c r="I65" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="40">
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="37"/>
+      <c r="O65" s="46">
         <v>44743</v>
       </c>
-      <c r="P65" s="40">
+      <c r="P65" s="46">
         <v>44749</v>
       </c>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-      <c r="S65" s="1"/>
-      <c r="T65" s="1"/>
-      <c r="U65" s="1"/>
-      <c r="V65" s="1"/>
-      <c r="W65" s="1"/>
-      <c r="X65" s="1"/>
-      <c r="Y65" s="1"/>
-      <c r="Z65" s="1"/>
-      <c r="AA65" s="1"/>
-      <c r="AB65" s="1"/>
-      <c r="AC65" s="1"/>
-      <c r="AD65" s="1"/>
-      <c r="AE65" s="1"/>
-      <c r="AF65" s="1"/>
-      <c r="AG65" s="1"/>
-      <c r="AH65" s="1"/>
-      <c r="AI65" s="1"/>
-      <c r="AJ65" s="1"/>
-      <c r="AK65" s="1"/>
-      <c r="AL65" s="1"/>
-      <c r="AM65" s="1"/>
-      <c r="AN65" s="1"/>
-      <c r="AO65" s="1"/>
-      <c r="AP65" s="1"/>
-      <c r="AQ65" s="1"/>
-      <c r="AR65" s="1"/>
-      <c r="AS65" s="1"/>
-      <c r="AT65" s="1" t="s">
+      <c r="Q65" s="37"/>
+      <c r="R65" s="37"/>
+      <c r="S65" s="37"/>
+      <c r="T65" s="37"/>
+      <c r="U65" s="37"/>
+      <c r="V65" s="37"/>
+      <c r="W65" s="37"/>
+      <c r="X65" s="37"/>
+      <c r="Y65" s="37"/>
+      <c r="Z65" s="37"/>
+      <c r="AA65" s="37"/>
+      <c r="AB65" s="37"/>
+      <c r="AC65" s="37"/>
+      <c r="AD65" s="37"/>
+      <c r="AE65" s="37"/>
+      <c r="AF65" s="37"/>
+      <c r="AG65" s="37"/>
+      <c r="AH65" s="37"/>
+      <c r="AI65" s="37"/>
+      <c r="AJ65" s="37"/>
+      <c r="AK65" s="37"/>
+      <c r="AL65" s="37"/>
+      <c r="AM65" s="37"/>
+      <c r="AN65" s="37"/>
+      <c r="AO65" s="37"/>
+      <c r="AP65" s="37"/>
+      <c r="AQ65" s="37"/>
+      <c r="AR65" s="37"/>
+      <c r="AS65" s="37"/>
+      <c r="AT65" s="37" t="s">
         <v>514</v>
       </c>
-      <c r="AU65" s="1"/>
-      <c r="AV65" s="1"/>
-      <c r="AW65" s="32"/>
-      <c r="AX65" s="1"/>
-      <c r="AY65" s="1">
+      <c r="AU65" s="37"/>
+      <c r="AV65" s="37"/>
+      <c r="AW65" s="38"/>
+      <c r="AX65" s="37"/>
+      <c r="AY65" s="37">
         <v>1</v>
       </c>
-      <c r="AZ65" s="1" t="s">
+      <c r="AZ65" s="37" t="s">
         <v>510</v>
       </c>
-      <c r="BA65" s="1" t="s">
+      <c r="BA65" s="37" t="s">
         <v>511</v>
       </c>
-      <c r="BB65" s="1">
+      <c r="BB65" s="37">
         <v>10</v>
       </c>
-      <c r="BC65" s="1">
+      <c r="BC65" s="37">
         <v>50</v>
       </c>
-      <c r="BD65" s="1"/>
-      <c r="BE65" s="1"/>
-      <c r="BF65" s="1"/>
-      <c r="BG65" s="1"/>
-      <c r="BH65" s="1"/>
-      <c r="BI65" s="1"/>
-      <c r="BJ65" s="1"/>
-      <c r="BK65" s="1"/>
-      <c r="BL65" s="1"/>
-      <c r="BM65" s="1"/>
-      <c r="BN65" s="1"/>
-      <c r="BO65" s="1"/>
-      <c r="BP65" s="1"/>
-      <c r="BQ65" s="1"/>
-      <c r="BR65" s="1"/>
-      <c r="BS65" s="1"/>
-      <c r="BT65" s="1"/>
-      <c r="BU65" s="1"/>
-      <c r="BV65" s="1"/>
-      <c r="BW65" s="1"/>
-      <c r="BX65" s="1"/>
-      <c r="BY65" s="1"/>
-      <c r="BZ65" s="1"/>
-      <c r="CA65" s="1"/>
-      <c r="CB65" s="1"/>
-      <c r="CC65" s="1"/>
-      <c r="CD65" s="1"/>
-      <c r="CE65" s="1"/>
-      <c r="CF65" s="1"/>
-      <c r="CG65" s="1"/>
-      <c r="CH65" s="1"/>
-      <c r="CI65" s="1"/>
-      <c r="CJ65" s="1"/>
-      <c r="CK65" s="1"/>
-      <c r="CL65" s="1"/>
-      <c r="CM65" s="1"/>
-      <c r="CN65" s="1"/>
-      <c r="CO65" s="1"/>
-      <c r="CP65" s="1"/>
-      <c r="CQ65" s="1"/>
-      <c r="CR65" s="35"/>
-      <c r="CS65" s="34"/>
-      <c r="CT65" s="36"/>
-      <c r="CU65" s="1"/>
+      <c r="BD65" s="37"/>
+      <c r="BE65" s="37"/>
+      <c r="BF65" s="37"/>
+      <c r="BG65" s="37"/>
+      <c r="BH65" s="37"/>
+      <c r="BI65" s="37"/>
+      <c r="BJ65" s="37"/>
+      <c r="BK65" s="37"/>
+      <c r="BL65" s="37"/>
+      <c r="BM65" s="37"/>
+      <c r="BN65" s="37"/>
+      <c r="BO65" s="37"/>
+      <c r="BP65" s="37"/>
+      <c r="BQ65" s="37"/>
+      <c r="BR65" s="37"/>
+      <c r="BS65" s="37"/>
+      <c r="BT65" s="37"/>
+      <c r="BU65" s="37"/>
+      <c r="BV65" s="37"/>
+      <c r="BW65" s="37"/>
+      <c r="BX65" s="37"/>
+      <c r="BY65" s="37"/>
+      <c r="BZ65" s="37"/>
+      <c r="CA65" s="37"/>
+      <c r="CB65" s="37"/>
+      <c r="CC65" s="37"/>
+      <c r="CD65" s="37"/>
+      <c r="CE65" s="37"/>
+      <c r="CF65" s="37"/>
+      <c r="CG65" s="37"/>
+      <c r="CH65" s="37"/>
+      <c r="CI65" s="37"/>
+      <c r="CJ65" s="37"/>
+      <c r="CK65" s="37"/>
+      <c r="CL65" s="37"/>
+      <c r="CM65" s="37"/>
+      <c r="CN65" s="37"/>
+      <c r="CO65" s="37"/>
+      <c r="CP65" s="37"/>
+      <c r="CQ65" s="37"/>
+      <c r="CR65" s="47"/>
+      <c r="CS65" s="48"/>
+      <c r="CT65" s="49"/>
+      <c r="CU65" s="37"/>
+    </row>
+    <row r="66" spans="1:99">
+      <c r="A66" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B66" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="45" t="s">
+        <v>518</v>
+      </c>
+      <c r="D66" s="45" t="s">
+        <v>486</v>
+      </c>
+      <c r="E66" s="45" t="s">
+        <v>243</v>
+      </c>
+      <c r="F66" s="45" t="s">
+        <v>519</v>
+      </c>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="67" t="s">
+        <v>503</v>
+      </c>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="40"/>
+      <c r="P66" s="40"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="1"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
+      <c r="Z66" s="1"/>
+      <c r="AA66" s="1"/>
+      <c r="AB66" s="1"/>
+      <c r="AC66" s="1"/>
+      <c r="AD66" s="1"/>
+      <c r="AE66" s="1"/>
+      <c r="AF66" s="1"/>
+      <c r="AG66" s="1"/>
+      <c r="AH66" s="1"/>
+      <c r="AI66" s="1"/>
+      <c r="AJ66" s="1"/>
+      <c r="AK66" s="1"/>
+      <c r="AL66" s="1"/>
+      <c r="AM66" s="1"/>
+      <c r="AN66" s="1"/>
+      <c r="AO66" s="1"/>
+      <c r="AP66" s="1"/>
+      <c r="AQ66" s="1"/>
+      <c r="AR66" s="1"/>
+      <c r="AS66" s="1"/>
+      <c r="AT66" s="1"/>
+      <c r="AU66" s="1"/>
+      <c r="AV66" s="1"/>
+      <c r="AW66" s="32"/>
+      <c r="AX66" s="1"/>
+      <c r="AY66" s="1"/>
+      <c r="AZ66" s="1"/>
+      <c r="BA66" s="1"/>
+      <c r="BB66" s="1"/>
+      <c r="BC66" s="1"/>
+      <c r="BD66" s="1"/>
+      <c r="BE66" s="1"/>
+      <c r="BF66" s="1"/>
+      <c r="BG66" s="1"/>
+      <c r="BH66" s="1"/>
+      <c r="BI66" s="1"/>
+      <c r="BJ66" s="1"/>
+      <c r="BK66" s="1"/>
+      <c r="BL66" s="1"/>
+      <c r="BM66" s="1"/>
+      <c r="BN66" s="1"/>
+      <c r="BO66" s="1"/>
+      <c r="BP66" s="1"/>
+      <c r="BQ66" s="1"/>
+      <c r="BR66" s="1"/>
+      <c r="BS66" s="1"/>
+      <c r="BT66" s="1"/>
+      <c r="BU66" s="1"/>
+      <c r="BV66" s="1"/>
+      <c r="BW66" s="1"/>
+      <c r="BX66" s="1"/>
+      <c r="BY66" s="1"/>
+      <c r="BZ66" s="1"/>
+      <c r="CA66" s="1"/>
+      <c r="CB66" s="1"/>
+      <c r="CC66" s="1"/>
+      <c r="CD66" s="1"/>
+      <c r="CE66" s="1"/>
+      <c r="CF66" s="1"/>
+      <c r="CG66" s="1"/>
+      <c r="CH66" s="1"/>
+      <c r="CI66" s="1"/>
+      <c r="CJ66" s="1"/>
+      <c r="CK66" s="1"/>
+      <c r="CL66" s="1"/>
+      <c r="CM66" s="1"/>
+      <c r="CN66" s="1"/>
+      <c r="CO66" s="1"/>
+      <c r="CP66" s="1"/>
+      <c r="CQ66" s="1"/>
+      <c r="CR66" s="35"/>
+      <c r="CS66" s="34"/>
+      <c r="CT66" s="36"/>
+      <c r="CU66" s="1"/>
+    </row>
+    <row r="67" spans="1:99">
+      <c r="A67" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B67" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="45" t="s">
+        <v>518</v>
+      </c>
+      <c r="D67" s="45" t="s">
+        <v>486</v>
+      </c>
+      <c r="E67" s="45" t="s">
+        <v>243</v>
+      </c>
+      <c r="F67" s="45" t="s">
+        <v>520</v>
+      </c>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="67" t="s">
+        <v>503</v>
+      </c>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="40"/>
+      <c r="P67" s="40"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="1"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
+      <c r="Z67" s="1"/>
+      <c r="AA67" s="1"/>
+      <c r="AB67" s="1"/>
+      <c r="AC67" s="1"/>
+      <c r="AD67" s="1"/>
+      <c r="AE67" s="1"/>
+      <c r="AF67" s="1"/>
+      <c r="AG67" s="1"/>
+      <c r="AH67" s="1"/>
+      <c r="AI67" s="1"/>
+      <c r="AJ67" s="1"/>
+      <c r="AK67" s="1"/>
+      <c r="AL67" s="1"/>
+      <c r="AM67" s="1"/>
+      <c r="AN67" s="1"/>
+      <c r="AO67" s="1"/>
+      <c r="AP67" s="1"/>
+      <c r="AQ67" s="1"/>
+      <c r="AR67" s="1"/>
+      <c r="AS67" s="1"/>
+      <c r="AT67" s="1"/>
+      <c r="AU67" s="1"/>
+      <c r="AV67" s="1"/>
+      <c r="AW67" s="32"/>
+      <c r="AX67" s="1"/>
+      <c r="AY67" s="1"/>
+      <c r="AZ67" s="1"/>
+      <c r="BA67" s="1"/>
+      <c r="BB67" s="1"/>
+      <c r="BC67" s="1"/>
+      <c r="BD67" s="1"/>
+      <c r="BE67" s="1"/>
+      <c r="BF67" s="1"/>
+      <c r="BG67" s="1"/>
+      <c r="BH67" s="1"/>
+      <c r="BI67" s="1"/>
+      <c r="BJ67" s="1"/>
+      <c r="BK67" s="1"/>
+      <c r="BL67" s="1"/>
+      <c r="BM67" s="1"/>
+      <c r="BN67" s="1"/>
+      <c r="BO67" s="1"/>
+      <c r="BP67" s="1"/>
+      <c r="BQ67" s="1"/>
+      <c r="BR67" s="1"/>
+      <c r="BS67" s="1"/>
+      <c r="BT67" s="1"/>
+      <c r="BU67" s="1"/>
+      <c r="BV67" s="1"/>
+      <c r="BW67" s="1"/>
+      <c r="BX67" s="1"/>
+      <c r="BY67" s="1"/>
+      <c r="BZ67" s="1"/>
+      <c r="CA67" s="1"/>
+      <c r="CB67" s="1"/>
+      <c r="CC67" s="1"/>
+      <c r="CD67" s="1"/>
+      <c r="CE67" s="1"/>
+      <c r="CF67" s="1"/>
+      <c r="CG67" s="1"/>
+      <c r="CH67" s="1"/>
+      <c r="CI67" s="1"/>
+      <c r="CJ67" s="1"/>
+      <c r="CK67" s="1"/>
+      <c r="CL67" s="1"/>
+      <c r="CM67" s="1"/>
+      <c r="CN67" s="1"/>
+      <c r="CO67" s="1"/>
+      <c r="CP67" s="1"/>
+      <c r="CQ67" s="1"/>
+      <c r="CR67" s="35"/>
+      <c r="CS67" s="34"/>
+      <c r="CT67" s="36"/>
+      <c r="CU67" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>